<commit_message>
Requirement Analysis is in progress
Requirement Analysis is in progress
</commit_message>
<xml_diff>
--- a/Offline/BusinessManagement/Website/Requirement-Analysis.xlsx
+++ b/Offline/BusinessManagement/Website/Requirement-Analysis.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Anodiam\Docs\Offline\BusinessManagement\Website\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60F03376-BA3E-4747-BFF9-B62F81C14846}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AI-Schools" sheetId="1" r:id="rId1"/>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="29">
   <si>
     <t>Slno</t>
   </si>
@@ -36,9 +37,6 @@
     <t>Parent</t>
   </si>
   <si>
-    <t>Where is Anodiam  located ?</t>
-  </si>
-  <si>
     <t>How many AI faculties are there ?</t>
   </si>
   <si>
@@ -84,13 +82,43 @@
     <t>Website(Y/N) ?</t>
   </si>
   <si>
-    <t>Student</t>
+    <t>Where is Anodiam  located (Address &amp; Phone Number) ?</t>
+  </si>
+  <si>
+    <t>Is Anodiam providing labs for AI ?</t>
+  </si>
+  <si>
+    <t>Is there any internal tests ?</t>
+  </si>
+  <si>
+    <t>Do Anodiam have any App ?</t>
+  </si>
+  <si>
+    <t>User</t>
+  </si>
+  <si>
+    <t>Do Anodiam provide course materials ?</t>
+  </si>
+  <si>
+    <t>Do Anodiam conduct online classes ?</t>
+  </si>
+  <si>
+    <t>After taking the course what is the prospect of my son/daughter ?</t>
+  </si>
+  <si>
+    <t>Principal</t>
+  </si>
+  <si>
+    <t>Will Anodiam conduct classes in school premises ?</t>
+  </si>
+  <si>
+    <t>What are the extra things Anodiam will provide to students other than AI ?</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -416,17 +444,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D15"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="A24" sqref="A24:A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="4.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="64.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.77734375" style="1" bestFit="1" customWidth="1"/>
   </cols>
@@ -436,13 +464,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
@@ -453,10 +481,10 @@
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>3</v>
+        <v>18</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -467,10 +495,10 @@
         <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
@@ -481,10 +509,10 @@
         <v>2</v>
       </c>
       <c r="C5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -495,10 +523,10 @@
         <v>2</v>
       </c>
       <c r="C6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
@@ -509,10 +537,10 @@
         <v>2</v>
       </c>
       <c r="C7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
@@ -523,10 +551,10 @@
         <v>2</v>
       </c>
       <c r="C8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
@@ -537,10 +565,10 @@
         <v>2</v>
       </c>
       <c r="C9" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
@@ -551,10 +579,10 @@
         <v>2</v>
       </c>
       <c r="C10" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
@@ -565,10 +593,10 @@
         <v>2</v>
       </c>
       <c r="C11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
@@ -579,10 +607,10 @@
         <v>2</v>
       </c>
       <c r="C12" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
@@ -593,10 +621,10 @@
         <v>2</v>
       </c>
       <c r="C13" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
@@ -607,10 +635,10 @@
         <v>2</v>
       </c>
       <c r="C14" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
@@ -621,19 +649,131 @@
         <v>2</v>
       </c>
       <c r="C15" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D15" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" s="1">
+        <v>14</v>
+      </c>
+      <c r="B16" t="s">
+        <v>2</v>
+      </c>
+      <c r="C16" t="s">
+        <v>19</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" s="1">
+        <v>15</v>
+      </c>
+      <c r="B17" t="s">
+        <v>2</v>
+      </c>
+      <c r="C17" t="s">
+        <v>20</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" s="1">
         <v>16</v>
+      </c>
+      <c r="B18" t="s">
+        <v>2</v>
+      </c>
+      <c r="C18" t="s">
+        <v>21</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" s="1">
+        <v>17</v>
+      </c>
+      <c r="B19" t="s">
+        <v>2</v>
+      </c>
+      <c r="C19" t="s">
+        <v>23</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" s="1">
+        <v>18</v>
+      </c>
+      <c r="B20" t="s">
+        <v>2</v>
+      </c>
+      <c r="C20" t="s">
+        <v>24</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" s="1">
+        <v>19</v>
+      </c>
+      <c r="B21" t="s">
+        <v>2</v>
+      </c>
+      <c r="C21" t="s">
+        <v>25</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" s="1">
+        <v>20</v>
+      </c>
+      <c r="B22" t="s">
+        <v>26</v>
+      </c>
+      <c r="C22" t="s">
+        <v>27</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23" s="1">
+        <v>21</v>
+      </c>
+      <c r="B23" t="s">
+        <v>26</v>
+      </c>
+      <c r="C23" t="s">
+        <v>28</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B1048576">
-      <formula1>"Parent,Student"</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1:B1048576" xr:uid="{00000000-0002-0000-0000-000001000000}">
+      <formula1>"Parent,Student,Principal,Teacher"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1">
-      <formula1>"Parent,Student,Principal"</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1:D1048576" xr:uid="{7207A645-9D0A-4BD8-909E-10728409CD8E}">
+      <formula1>"Y,N"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -641,7 +781,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>